<commit_message>
add order changing status
</commit_message>
<xml_diff>
--- a/application/handlers/database/orders.xlsx
+++ b/application/handlers/database/orders.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Дата</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>KZT</t>
+  </si>
+  <si>
+    <t>payed</t>
   </si>
   <si>
     <t>https://www.zara.com/kz/ru/share/-p01131888.html?utm_campaign=productShare&amp;utm_medium=mobile_sharing_iOS&amp;utm_source=red_social_movil&amp;v1=204986543</t>
@@ -594,10 +597,10 @@
         <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>